<commit_message>
Last template provided by Anthony.
</commit_message>
<xml_diff>
--- a/CE301_grades/template_second_assessor.xlsx
+++ b/CE301_grades/template_second_assessor.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthony/Documents/OneDriveBusiness/Education/2015-16/Teaching/CE301/Assessments/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23800" windowHeight="19940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23800" windowHeight="19940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Second Assessor Mark Form" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -96,9 +101,6 @@
     <t>Technical quality of verbal responses</t>
   </si>
   <si>
-    <t>CE301 FINAL YEAR PROJECT - SECOND ASSESSOR MARK FORM 2014-15</t>
-  </si>
-  <si>
     <t>Weighted range</t>
   </si>
   <si>
@@ -139,6 +141,9 @@
   </si>
   <si>
     <t>PDO (15%)</t>
+  </si>
+  <si>
+    <t>CE301 FINAL YEAR PROJECT - SECOND ASSESSOR MARK FORM 2015-16</t>
   </si>
 </sst>
 </file>
@@ -151,7 +156,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -514,26 +518,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -553,10 +537,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -570,6 +574,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -901,10 +910,10 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="48.5" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
@@ -913,105 +922,105 @@
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="26"/>
-      <c r="B1" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="27"/>
-      <c r="B2" s="23"/>
+    <row r="1" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="20"/>
+      <c r="B1" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="21"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="27"/>
-      <c r="B3" s="24" t="s">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="21"/>
+      <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
-      <c r="A4" s="27"/>
-      <c r="B4" s="24" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21"/>
+      <c r="B4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
-      <c r="A5" s="27"/>
-      <c r="B5" s="24" t="s">
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21"/>
+      <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
-      <c r="A6" s="27"/>
-      <c r="B6" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="27"/>
-      <c r="B7" s="23"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="30"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21"/>
+      <c r="B6" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="21"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="27"/>
-      <c r="B8" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:6" ht="30">
-      <c r="A9" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="21" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="21"/>
+      <c r="B8" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="26"/>
+    </row>
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="29"/>
-      <c r="B10" s="22" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
+      <c r="B10" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="3">
@@ -1028,9 +1037,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="29"/>
-      <c r="B11" s="22" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3">
@@ -1047,9 +1056,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="29"/>
-      <c r="B12" s="22" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="24"/>
+      <c r="B12" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="3">
@@ -1066,9 +1075,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="29"/>
-      <c r="B13" s="22"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="24"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="2"/>
       <c r="D13" s="8"/>
       <c r="E13" s="1" t="s">
@@ -1079,40 +1088,40 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="30"/>
-      <c r="B14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:6" ht="30">
-      <c r="A15" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="21" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="23"/>
+      <c r="B14" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26"/>
+    </row>
+    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="29"/>
-      <c r="B16" s="22" t="s">
-        <v>30</v>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="24"/>
+      <c r="B16" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="C16" s="3">
         <v>100</v>
@@ -1128,10 +1137,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="29"/>
-      <c r="B17" s="22" t="s">
-        <v>31</v>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="24"/>
+      <c r="B17" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="C17" s="3">
         <v>100</v>
@@ -1147,9 +1156,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="29"/>
-      <c r="B18" s="22" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+      <c r="B18" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="3">
@@ -1166,9 +1175,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="29"/>
-      <c r="B19" s="22" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="24"/>
+      <c r="B19" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="3">
@@ -1185,9 +1194,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="29"/>
-      <c r="B20" s="22"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="24"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="2"/>
       <c r="D20" s="8"/>
       <c r="E20" s="1" t="s">
@@ -1198,39 +1207,39 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="30"/>
-      <c r="B21" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="1:6" ht="30">
-      <c r="A22" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="21" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="23"/>
+      <c r="B21" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="26"/>
+    </row>
+    <row r="22" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="29"/>
-      <c r="B23" s="22" t="s">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="24"/>
+      <c r="B23" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="3">
@@ -1247,9 +1256,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="29"/>
-      <c r="B24" s="22" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="24"/>
+      <c r="B24" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="3">
@@ -1266,9 +1275,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="29"/>
-      <c r="B25" s="22" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="24"/>
+      <c r="B25" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="3">
@@ -1285,9 +1294,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="29"/>
-      <c r="B26" s="22"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="24"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="2"/>
       <c r="D26" s="8"/>
       <c r="E26" s="1" t="s">
@@ -1298,39 +1307,39 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="30"/>
-      <c r="B27" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="1:6" ht="30">
-      <c r="A28" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="21" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="23"/>
+      <c r="B27" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="26"/>
+    </row>
+    <row r="28" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="29"/>
-      <c r="B29" s="22" t="s">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="24"/>
+      <c r="B29" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="3">
@@ -1347,9 +1356,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="29"/>
-      <c r="B30" s="22" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="24"/>
+      <c r="B30" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C30" s="3">
@@ -1366,9 +1375,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="29"/>
-      <c r="B31" s="22" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="24"/>
+      <c r="B31" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C31" s="3">
@@ -1385,9 +1394,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="29"/>
-      <c r="B32" s="22" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="24"/>
+      <c r="B32" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C32" s="3">
@@ -1404,9 +1413,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16" thickBot="1">
-      <c r="A33" s="28"/>
-      <c r="B33" s="25"/>
+    <row r="33" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="9"/>
       <c r="D33" s="10"/>
       <c r="E33" s="11" t="s">
@@ -1420,6 +1429,12 @@
   </sheetData>
   <sheetProtection password="F68B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="A22:A26"/>
@@ -1427,20 +1442,9 @@
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="B8:F8"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="79" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>